<commit_message>
added sports.xlsx to codes
</commit_message>
<xml_diff>
--- a/data/1_input/Sports/sports.xlsx
+++ b/data/1_input/Sports/sports.xlsx
@@ -5,22 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cheekeet\OneDrive\Work\GA DSI\Lab\working-directory\project-capstone\data\1_input\FitRec\sports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cheekeet\OneDrive\Work\GA DSI\Lab\working-directory\project-capstone\data\1_input\Sports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02812196-07EE-421B-AAD6-EF549BE70588}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="102_{DC91454B-DDAA-49F8-BA64-9DB9F9AA9C15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{7DE89CA3-250B-46D2-A0BC-DA867A0CEF31}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sports" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sports!$A$1:$H$44</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="66">
   <si>
     <t>run</t>
   </si>
@@ -154,30 +157,9 @@
     <t>gentlemen</t>
   </si>
   <si>
-    <t>distance</t>
-  </si>
-  <si>
-    <t>speed</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>valid</t>
-  </si>
-  <si>
-    <t>invalid</t>
-  </si>
-  <si>
     <t>gym</t>
   </si>
   <si>
-    <t>sport_original</t>
-  </si>
-  <si>
-    <t>sport_combined</t>
-  </si>
-  <si>
     <t>speed_max</t>
   </si>
   <si>
@@ -224,6 +206,21 @@
   </si>
   <si>
     <t>rowing</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t>sport_rename</t>
+  </si>
+  <si>
+    <t>location_valid</t>
+  </si>
+  <si>
+    <t>distance_valid</t>
+  </si>
+  <si>
+    <t>speed_valid</t>
   </si>
 </sst>
 </file>
@@ -1089,8 +1086,8 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,18 +1095,18 @@
     <col min="1" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -1118,39 +1115,39 @@
         <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1169,14 +1166,14 @@
       <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1184,10 +1181,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -1195,14 +1192,14 @@
       <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1221,14 +1218,14 @@
       <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" t="s">
-        <v>47</v>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
       </c>
       <c r="H5">
         <v>244</v>
@@ -1247,14 +1244,14 @@
       <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" t="s">
-        <v>47</v>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
       </c>
       <c r="H6">
         <v>244</v>
@@ -1273,14 +1270,14 @@
       <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" t="s">
-        <v>47</v>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
       </c>
       <c r="H7">
         <v>244</v>
@@ -1299,14 +1296,14 @@
       <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" t="s">
-        <v>47</v>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
       </c>
       <c r="H8">
         <v>244</v>
@@ -1314,10 +1311,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -1325,14 +1322,14 @@
       <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" t="s">
-        <v>48</v>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1340,10 +1337,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -1351,14 +1348,14 @@
       <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1366,10 +1363,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -1377,14 +1374,14 @@
       <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>48</v>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1398,19 +1395,19 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>48</v>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1418,10 +1415,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>43</v>
@@ -1429,14 +1426,14 @@
       <c r="D13" t="s">
         <v>42</v>
       </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" t="s">
-        <v>48</v>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1455,14 +1452,14 @@
       <c r="D14" t="s">
         <v>38</v>
       </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" t="s">
-        <v>48</v>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1481,14 +1478,14 @@
       <c r="D15" t="s">
         <v>42</v>
       </c>
-      <c r="E15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" t="s">
-        <v>47</v>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
       </c>
       <c r="H15">
         <v>45</v>
@@ -1507,14 +1504,14 @@
       <c r="D16" t="s">
         <v>42</v>
       </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" t="s">
-        <v>47</v>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
       </c>
       <c r="H16">
         <v>71</v>
@@ -1533,14 +1530,14 @@
       <c r="D17" t="s">
         <v>36</v>
       </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" t="s">
-        <v>47</v>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
       </c>
       <c r="H17">
         <v>32</v>
@@ -1559,14 +1556,14 @@
       <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="E18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" t="s">
-        <v>48</v>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1585,14 +1582,14 @@
       <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" t="s">
-        <v>47</v>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
       </c>
       <c r="H19">
         <v>45</v>
@@ -1600,10 +1597,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
         <v>36</v>
@@ -1611,14 +1608,14 @@
       <c r="D20" t="s">
         <v>36</v>
       </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" t="s">
-        <v>47</v>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
       </c>
       <c r="H20">
         <v>23</v>
@@ -1626,10 +1623,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
@@ -1637,14 +1634,14 @@
       <c r="D21" t="s">
         <v>42</v>
       </c>
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" t="s">
-        <v>48</v>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1663,14 +1660,14 @@
       <c r="D22" t="s">
         <v>41</v>
       </c>
-      <c r="E22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" t="s">
-        <v>47</v>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
       </c>
       <c r="H22">
         <v>45</v>
@@ -1689,14 +1686,14 @@
       <c r="D23" t="s">
         <v>38</v>
       </c>
-      <c r="E23" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" t="s">
-        <v>47</v>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
       </c>
       <c r="H23">
         <v>45</v>
@@ -1704,10 +1701,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
         <v>36</v>
@@ -1715,14 +1712,14 @@
       <c r="D24" t="s">
         <v>36</v>
       </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" t="s">
-        <v>47</v>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
       </c>
       <c r="H24">
         <v>121</v>
@@ -1741,14 +1738,14 @@
       <c r="D25" t="s">
         <v>41</v>
       </c>
-      <c r="E25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" t="s">
-        <v>47</v>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
       </c>
       <c r="H25">
         <v>55</v>
@@ -1767,14 +1764,14 @@
       <c r="D26" t="s">
         <v>37</v>
       </c>
-      <c r="E26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>47</v>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
       </c>
       <c r="H26">
         <v>255</v>
@@ -1793,14 +1790,14 @@
       <c r="D27" t="s">
         <v>37</v>
       </c>
-      <c r="E27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" t="s">
-        <v>47</v>
-      </c>
-      <c r="G27" t="s">
-        <v>47</v>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
       </c>
       <c r="H27">
         <v>255</v>
@@ -1819,14 +1816,14 @@
       <c r="D28" t="s">
         <v>41</v>
       </c>
-      <c r="E28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" t="s">
-        <v>47</v>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
       </c>
       <c r="H28">
         <v>50</v>
@@ -1845,14 +1842,14 @@
       <c r="D29" t="s">
         <v>37</v>
       </c>
-      <c r="E29" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" t="s">
-        <v>47</v>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
       </c>
       <c r="H29">
         <v>203</v>
@@ -1860,10 +1857,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
         <v>37</v>
@@ -1871,14 +1868,14 @@
       <c r="D30" t="s">
         <v>37</v>
       </c>
-      <c r="E30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" t="s">
-        <v>47</v>
-      </c>
-      <c r="G30" t="s">
-        <v>47</v>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
       </c>
       <c r="H30">
         <v>45</v>
@@ -1886,10 +1883,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
@@ -1897,14 +1894,14 @@
       <c r="D31" t="s">
         <v>42</v>
       </c>
-      <c r="E31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" t="s">
-        <v>48</v>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1912,10 +1909,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
         <v>35</v>
@@ -1923,14 +1920,14 @@
       <c r="D32" t="s">
         <v>38</v>
       </c>
-      <c r="E32" t="s">
-        <v>48</v>
-      </c>
-      <c r="F32" t="s">
-        <v>47</v>
-      </c>
-      <c r="G32" t="s">
-        <v>48</v>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -1941,7 +1938,7 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
         <v>34</v>
@@ -1949,14 +1946,14 @@
       <c r="D33" t="s">
         <v>41</v>
       </c>
-      <c r="E33" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" t="s">
-        <v>48</v>
-      </c>
-      <c r="G33" t="s">
-        <v>48</v>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1975,14 +1972,14 @@
       <c r="D34" t="s">
         <v>36</v>
       </c>
-      <c r="E34" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" t="s">
-        <v>47</v>
-      </c>
-      <c r="G34" t="s">
-        <v>47</v>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
       </c>
       <c r="H34">
         <v>99</v>
@@ -2001,14 +1998,14 @@
       <c r="D35" t="s">
         <v>36</v>
       </c>
-      <c r="E35" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G35" t="s">
-        <v>47</v>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
       </c>
       <c r="H35">
         <v>99</v>
@@ -2027,14 +2024,14 @@
       <c r="D36" t="s">
         <v>36</v>
       </c>
-      <c r="E36" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" t="s">
-        <v>47</v>
-      </c>
-      <c r="G36" t="s">
-        <v>47</v>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
       </c>
       <c r="H36">
         <v>9</v>
@@ -2053,14 +2050,14 @@
       <c r="D37" t="s">
         <v>38</v>
       </c>
-      <c r="E37" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G37" t="s">
-        <v>48</v>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -2079,14 +2076,14 @@
       <c r="D38" t="s">
         <v>42</v>
       </c>
-      <c r="E38" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" t="s">
-        <v>47</v>
-      </c>
-      <c r="G38" t="s">
-        <v>48</v>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2105,14 +2102,14 @@
       <c r="D39" t="s">
         <v>41</v>
       </c>
-      <c r="E39" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" t="s">
-        <v>47</v>
-      </c>
-      <c r="G39" t="s">
-        <v>47</v>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
       </c>
       <c r="H39">
         <v>45</v>
@@ -2131,14 +2128,14 @@
       <c r="D40" t="s">
         <v>38</v>
       </c>
-      <c r="E40" t="s">
-        <v>48</v>
-      </c>
-      <c r="F40" t="s">
-        <v>47</v>
-      </c>
-      <c r="G40" t="s">
-        <v>47</v>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
       </c>
       <c r="H40">
         <v>45</v>
@@ -2157,14 +2154,14 @@
       <c r="D41" t="s">
         <v>41</v>
       </c>
-      <c r="E41" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" t="s">
-        <v>47</v>
-      </c>
-      <c r="G41" t="s">
-        <v>47</v>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
       </c>
       <c r="H41">
         <v>45</v>
@@ -2178,19 +2175,19 @@
         <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D42" t="s">
         <v>38</v>
       </c>
-      <c r="E42" t="s">
-        <v>48</v>
-      </c>
-      <c r="F42" t="s">
-        <v>48</v>
-      </c>
-      <c r="G42" t="s">
-        <v>48</v>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -2209,14 +2206,14 @@
       <c r="D43" t="s">
         <v>38</v>
       </c>
-      <c r="E43" t="s">
-        <v>48</v>
-      </c>
-      <c r="F43" t="s">
-        <v>48</v>
-      </c>
-      <c r="G43" t="s">
-        <v>48</v>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -2235,14 +2232,14 @@
       <c r="D44" t="s">
         <v>38</v>
       </c>
-      <c r="E44" t="s">
-        <v>48</v>
-      </c>
-      <c r="F44" t="s">
-        <v>48</v>
-      </c>
-      <c r="G44" t="s">
-        <v>48</v>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -2255,10 +2252,10 @@
   </sortState>
   <conditionalFormatting sqref="E1:G1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"invalid"</formula>
+      <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"valid"</formula>
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>